<commit_message>
Add more fuel switching and process emission capture for the cement industry
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_IND_Emi_Proc_BASE.xlsx
+++ b/SuppXLS/Scen_IND_Emi_Proc_BASE.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\E4SMA-7\Documents\E4SMA Collaborazioni\UCC\2021.02-03_IND mitigation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6684D0CE-A2B0-444F-A20B-0C971CCA320E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB453989-3EF2-4E6C-8216-0BEE417A6A22}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="78">
   <si>
     <t>Development</t>
   </si>
@@ -316,13 +316,25 @@
   <si>
     <t>FLO_EMIS</t>
   </si>
+  <si>
+    <t>I-DMD-ONM-N1</t>
+  </si>
+  <si>
+    <t>*CCS option</t>
+  </si>
+  <si>
+    <t>Capture rate</t>
+  </si>
+  <si>
+    <t>INDCO2S</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="\Te\x\t"/>
+    <numFmt numFmtId="164" formatCode="\Te\x\t"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -392,7 +404,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -443,6 +455,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -552,7 +570,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -570,17 +588,17 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="3" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -593,6 +611,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="a_Calc_Outputs" xfId="2" xr:uid="{BDC6809B-EE47-49A8-B3E8-0AF2A0A5AA06}"/>
@@ -642,7 +668,7 @@
                   <a14:compatExt spid="_x0000_s1025"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1709,10 +1735,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BB24379-873C-4F8C-A76D-60FB935DBEAA}">
-  <dimension ref="B1:O53"/>
+  <dimension ref="B1:O110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q23" sqref="Q23"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I68" sqref="I68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2506,7 +2532,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B33" s="1"/>
       <c r="C33" s="11"/>
       <c r="D33" s="1" t="s">
@@ -2532,7 +2558,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
       <c r="C34" s="11"/>
       <c r="D34" s="1" t="s">
@@ -2558,7 +2584,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B35" s="1"/>
       <c r="C35" s="11"/>
       <c r="D35" s="1" t="s">
@@ -2584,7 +2610,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
       <c r="C36" s="11"/>
       <c r="D36" s="1" t="s">
@@ -2610,7 +2636,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B37" s="1"/>
       <c r="C37" s="11"/>
       <c r="D37" s="1" t="s">
@@ -2636,7 +2662,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B38" s="1"/>
       <c r="C38" s="11"/>
       <c r="D38" s="1" t="s">
@@ -2662,76 +2688,1812 @@
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B39" s="1"/>
-      <c r="C39" s="11"/>
-      <c r="D39" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E39" s="1">
+    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B39" s="10"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E39" s="10">
         <v>2100</v>
       </c>
-      <c r="F39" s="9">
+      <c r="F39" s="23">
         <v>129.72050850162699</v>
       </c>
-      <c r="G39" s="9">
+      <c r="G39" s="23">
         <f t="shared" si="0"/>
         <v>129.72050850162699</v>
       </c>
-      <c r="H39" s="8" t="s">
+      <c r="H39" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="I39" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="J39" s="20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I39" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="J39" s="25" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B40" s="21" t="s">
+        <v>75</v>
+      </c>
       <c r="C40" s="11"/>
-    </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="L40" s="21" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C41" s="11"/>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D41" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E41" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F41" s="9">
+        <f>F5*(1-$L$41)</f>
+        <v>8.2460032276080835</v>
+      </c>
+      <c r="G41" s="9">
+        <f>F41</f>
+        <v>8.2460032276080835</v>
+      </c>
+      <c r="H41" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I41" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J41" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="L41" s="26">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C42" s="11"/>
-    </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D42" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E42" s="1">
+        <v>2019</v>
+      </c>
+      <c r="F42" s="9">
+        <f t="shared" ref="F42:F105" si="1">F6*(1-$L$41)</f>
+        <v>7.7562180785042045</v>
+      </c>
+      <c r="G42" s="9">
+        <f t="shared" ref="G42:G75" si="2">F42</f>
+        <v>7.7562180785042045</v>
+      </c>
+      <c r="H42" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I42" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J42" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C43" s="11"/>
-    </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D43" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E43" s="1">
+        <v>2020</v>
+      </c>
+      <c r="F43" s="9">
+        <f t="shared" si="1"/>
+        <v>8.872035169299183</v>
+      </c>
+      <c r="G43" s="9">
+        <f t="shared" si="2"/>
+        <v>8.872035169299183</v>
+      </c>
+      <c r="H43" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I43" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J43" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C44" s="11"/>
-    </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D44" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E44" s="1">
+        <v>2021</v>
+      </c>
+      <c r="F44" s="9">
+        <f t="shared" si="1"/>
+        <v>9.1930668300077549</v>
+      </c>
+      <c r="G44" s="9">
+        <f t="shared" si="2"/>
+        <v>9.1930668300077549</v>
+      </c>
+      <c r="H44" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I44" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J44" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C45" s="11"/>
-    </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D45" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E45" s="1">
+        <v>2022</v>
+      </c>
+      <c r="F45" s="9">
+        <f t="shared" si="1"/>
+        <v>9.3648044164639224</v>
+      </c>
+      <c r="G45" s="9">
+        <f t="shared" si="2"/>
+        <v>9.3648044164639224</v>
+      </c>
+      <c r="H45" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I45" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J45" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C46" s="11"/>
-    </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D46" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E46" s="1">
+        <v>2023</v>
+      </c>
+      <c r="F46" s="9">
+        <f t="shared" si="1"/>
+        <v>9.1160774382009446</v>
+      </c>
+      <c r="G46" s="9">
+        <f t="shared" si="2"/>
+        <v>9.1160774382009446</v>
+      </c>
+      <c r="H46" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I46" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J46" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C47" s="11"/>
-    </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D47" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E47" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F47" s="9">
+        <f t="shared" si="1"/>
+        <v>8.8810504968707136</v>
+      </c>
+      <c r="G47" s="9">
+        <f t="shared" si="2"/>
+        <v>8.8810504968707136</v>
+      </c>
+      <c r="H47" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I47" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J47" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C48" s="11"/>
-    </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D48" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E48" s="1">
+        <v>2025</v>
+      </c>
+      <c r="F48" s="9">
+        <f t="shared" si="1"/>
+        <v>8.7200521554827031</v>
+      </c>
+      <c r="G48" s="9">
+        <f t="shared" si="2"/>
+        <v>8.7200521554827031</v>
+      </c>
+      <c r="H48" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I48" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J48" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="49" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C49" s="11"/>
-    </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D49" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E49" s="1">
+        <v>2026</v>
+      </c>
+      <c r="F49" s="9">
+        <f t="shared" si="1"/>
+        <v>8.5897110384340447</v>
+      </c>
+      <c r="G49" s="9">
+        <f t="shared" si="2"/>
+        <v>8.5897110384340447</v>
+      </c>
+      <c r="H49" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I49" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J49" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="50" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C50" s="11"/>
-    </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D50" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E50" s="1">
+        <v>2027</v>
+      </c>
+      <c r="F50" s="9">
+        <f t="shared" si="1"/>
+        <v>8.4828508985189135</v>
+      </c>
+      <c r="G50" s="9">
+        <f t="shared" si="2"/>
+        <v>8.4828508985189135</v>
+      </c>
+      <c r="H50" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I50" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J50" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="51" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C51" s="11"/>
-    </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D51" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E51" s="1">
+        <v>2028</v>
+      </c>
+      <c r="F51" s="9">
+        <f t="shared" si="1"/>
+        <v>8.3925807369767949</v>
+      </c>
+      <c r="G51" s="9">
+        <f t="shared" si="2"/>
+        <v>8.3925807369767949</v>
+      </c>
+      <c r="H51" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I51" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J51" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="52" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C52" s="11"/>
-    </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D52" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E52" s="1">
+        <v>2029</v>
+      </c>
+      <c r="F52" s="9">
+        <f t="shared" si="1"/>
+        <v>8.3027057053633637</v>
+      </c>
+      <c r="G52" s="9">
+        <f t="shared" si="2"/>
+        <v>8.3027057053633637</v>
+      </c>
+      <c r="H52" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I52" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J52" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="53" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C53" s="11"/>
+      <c r="D53" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E53" s="1">
+        <v>2030</v>
+      </c>
+      <c r="F53" s="9">
+        <f t="shared" si="1"/>
+        <v>8.2134413129550534</v>
+      </c>
+      <c r="G53" s="9">
+        <f t="shared" si="2"/>
+        <v>8.2134413129550534</v>
+      </c>
+      <c r="H53" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I53" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J53" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="54" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D54" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E54" s="1">
+        <v>2031</v>
+      </c>
+      <c r="F54" s="9">
+        <f t="shared" si="1"/>
+        <v>8.4821784144071053</v>
+      </c>
+      <c r="G54" s="9">
+        <f t="shared" si="2"/>
+        <v>8.4821784144071053</v>
+      </c>
+      <c r="H54" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I54" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J54" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="55" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D55" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E55" s="1">
+        <v>2032</v>
+      </c>
+      <c r="F55" s="9">
+        <f t="shared" si="1"/>
+        <v>8.1722103165168836</v>
+      </c>
+      <c r="G55" s="9">
+        <f t="shared" si="2"/>
+        <v>8.1722103165168836</v>
+      </c>
+      <c r="H55" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I55" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J55" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="56" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D56" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E56" s="1">
+        <v>2033</v>
+      </c>
+      <c r="F56" s="9">
+        <f t="shared" si="1"/>
+        <v>8.0920889656202348</v>
+      </c>
+      <c r="G56" s="9">
+        <f t="shared" si="2"/>
+        <v>8.0920889656202348</v>
+      </c>
+      <c r="H56" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I56" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J56" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="57" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D57" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E57" s="1">
+        <v>2034</v>
+      </c>
+      <c r="F57" s="9">
+        <f t="shared" si="1"/>
+        <v>8.0133390674843739</v>
+      </c>
+      <c r="G57" s="9">
+        <f t="shared" si="2"/>
+        <v>8.0133390674843739</v>
+      </c>
+      <c r="H57" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I57" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J57" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="58" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D58" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E58" s="1">
+        <v>2035</v>
+      </c>
+      <c r="F58" s="9">
+        <f t="shared" si="1"/>
+        <v>7.9313085428571348</v>
+      </c>
+      <c r="G58" s="9">
+        <f t="shared" si="2"/>
+        <v>7.9313085428571348</v>
+      </c>
+      <c r="H58" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I58" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J58" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="59" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D59" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E59" s="1">
+        <v>2036</v>
+      </c>
+      <c r="F59" s="9">
+        <f t="shared" si="1"/>
+        <v>7.848091272568114</v>
+      </c>
+      <c r="G59" s="9">
+        <f t="shared" si="2"/>
+        <v>7.848091272568114</v>
+      </c>
+      <c r="H59" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I59" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J59" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="60" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D60" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E60" s="1">
+        <v>2037</v>
+      </c>
+      <c r="F60" s="9">
+        <f t="shared" si="1"/>
+        <v>7.7636033743134938</v>
+      </c>
+      <c r="G60" s="9">
+        <f t="shared" si="2"/>
+        <v>7.7636033743134938</v>
+      </c>
+      <c r="H60" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I60" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J60" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="61" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D61" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E61" s="1">
+        <v>2038</v>
+      </c>
+      <c r="F61" s="9">
+        <f t="shared" si="1"/>
+        <v>7.6787091840046653</v>
+      </c>
+      <c r="G61" s="9">
+        <f t="shared" si="2"/>
+        <v>7.6787091840046653</v>
+      </c>
+      <c r="H61" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I61" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J61" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="62" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D62" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E62" s="1">
+        <v>2039</v>
+      </c>
+      <c r="F62" s="9">
+        <f t="shared" si="1"/>
+        <v>7.5913619213730854</v>
+      </c>
+      <c r="G62" s="9">
+        <f t="shared" si="2"/>
+        <v>7.5913619213730854</v>
+      </c>
+      <c r="H62" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I62" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J62" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="63" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D63" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E63" s="1">
+        <v>2040</v>
+      </c>
+      <c r="F63" s="9">
+        <f t="shared" si="1"/>
+        <v>7.5031348909904052</v>
+      </c>
+      <c r="G63" s="9">
+        <f t="shared" si="2"/>
+        <v>7.5031348909904052</v>
+      </c>
+      <c r="H63" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I63" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J63" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="64" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D64" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E64" s="1">
+        <v>2045</v>
+      </c>
+      <c r="F64" s="9">
+        <f t="shared" si="1"/>
+        <v>12.851370744393501</v>
+      </c>
+      <c r="G64" s="9">
+        <f t="shared" si="2"/>
+        <v>12.851370744393501</v>
+      </c>
+      <c r="H64" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I64" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J64" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D65" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E65" s="1">
+        <v>2050</v>
+      </c>
+      <c r="F65" s="9">
+        <f t="shared" si="1"/>
+        <v>10.856813483392791</v>
+      </c>
+      <c r="G65" s="9">
+        <f t="shared" si="2"/>
+        <v>10.856813483392791</v>
+      </c>
+      <c r="H65" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I65" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J65" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D66" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E66" s="1">
+        <v>2055</v>
+      </c>
+      <c r="F66" s="9">
+        <f t="shared" si="1"/>
+        <v>10.144010025262533</v>
+      </c>
+      <c r="G66" s="9">
+        <f t="shared" si="2"/>
+        <v>10.144010025262533</v>
+      </c>
+      <c r="H66" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I66" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J66" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="67" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D67" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E67" s="1">
+        <v>2060</v>
+      </c>
+      <c r="F67" s="9">
+        <f t="shared" si="1"/>
+        <v>9.4128946391141142</v>
+      </c>
+      <c r="G67" s="9">
+        <f t="shared" si="2"/>
+        <v>9.4128946391141142</v>
+      </c>
+      <c r="H67" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I67" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J67" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="68" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D68" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E68" s="1">
+        <v>2065</v>
+      </c>
+      <c r="F68" s="9">
+        <f t="shared" si="1"/>
+        <v>9.4482495534202933</v>
+      </c>
+      <c r="G68" s="9">
+        <f t="shared" si="2"/>
+        <v>9.4482495534202933</v>
+      </c>
+      <c r="H68" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I68" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J68" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="69" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D69" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E69" s="1">
+        <v>2070</v>
+      </c>
+      <c r="F69" s="9">
+        <f t="shared" si="1"/>
+        <v>9.4048483031768235</v>
+      </c>
+      <c r="G69" s="9">
+        <f t="shared" si="2"/>
+        <v>9.4048483031768235</v>
+      </c>
+      <c r="H69" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I69" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J69" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D70" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E70" s="1">
+        <v>2075</v>
+      </c>
+      <c r="F70" s="9">
+        <f t="shared" si="1"/>
+        <v>9.4429755346118434</v>
+      </c>
+      <c r="G70" s="9">
+        <f t="shared" si="2"/>
+        <v>9.4429755346118434</v>
+      </c>
+      <c r="H70" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I70" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J70" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="71" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D71" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E71" s="1">
+        <v>2080</v>
+      </c>
+      <c r="F71" s="9">
+        <f t="shared" si="1"/>
+        <v>9.5143057194781324</v>
+      </c>
+      <c r="G71" s="9">
+        <f t="shared" si="2"/>
+        <v>9.5143057194781324</v>
+      </c>
+      <c r="H71" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I71" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J71" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="72" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D72" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E72" s="1">
+        <v>2085</v>
+      </c>
+      <c r="F72" s="9">
+        <f t="shared" si="1"/>
+        <v>9.5335037528884232</v>
+      </c>
+      <c r="G72" s="9">
+        <f t="shared" si="2"/>
+        <v>9.5335037528884232</v>
+      </c>
+      <c r="H72" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I72" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J72" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="73" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D73" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E73" s="1">
+        <v>2090</v>
+      </c>
+      <c r="F73" s="9">
+        <f t="shared" si="1"/>
+        <v>9.4616883688176436</v>
+      </c>
+      <c r="G73" s="9">
+        <f t="shared" si="2"/>
+        <v>9.4616883688176436</v>
+      </c>
+      <c r="H73" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I73" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J73" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="74" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D74" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E74" s="1">
+        <v>2095</v>
+      </c>
+      <c r="F74" s="9">
+        <f t="shared" si="1"/>
+        <v>9.2918387001078031</v>
+      </c>
+      <c r="G74" s="9">
+        <f t="shared" si="2"/>
+        <v>9.2918387001078031</v>
+      </c>
+      <c r="H74" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I74" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J74" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="75" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B75" s="10"/>
+      <c r="C75" s="10"/>
+      <c r="D75" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E75" s="10">
+        <v>2100</v>
+      </c>
+      <c r="F75" s="23">
+        <f t="shared" si="1"/>
+        <v>9.0804355951138831</v>
+      </c>
+      <c r="G75" s="23">
+        <f t="shared" si="2"/>
+        <v>9.0804355951138831</v>
+      </c>
+      <c r="H75" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="I75" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="J75" s="25" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="76" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D76" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E76" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F76" s="9">
+        <f>F5*$L$41</f>
+        <v>109.55404288107891</v>
+      </c>
+      <c r="G76" s="9">
+        <f>F76</f>
+        <v>109.55404288107891</v>
+      </c>
+      <c r="H76" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I76" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J76" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="77" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D77" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E77" s="1">
+        <v>2019</v>
+      </c>
+      <c r="F77" s="9">
+        <f t="shared" ref="F77:F110" si="3">F6*$L$41</f>
+        <v>103.04689732869879</v>
+      </c>
+      <c r="G77" s="9">
+        <f t="shared" ref="G77:G110" si="4">F77</f>
+        <v>103.04689732869879</v>
+      </c>
+      <c r="H77" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I77" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J77" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="78" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D78" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E78" s="1">
+        <v>2020</v>
+      </c>
+      <c r="F78" s="9">
+        <f t="shared" si="3"/>
+        <v>117.87132439211781</v>
+      </c>
+      <c r="G78" s="9">
+        <f t="shared" si="4"/>
+        <v>117.87132439211781</v>
+      </c>
+      <c r="H78" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I78" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J78" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="79" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D79" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E79" s="1">
+        <v>2021</v>
+      </c>
+      <c r="F79" s="9">
+        <f t="shared" si="3"/>
+        <v>122.13645931296026</v>
+      </c>
+      <c r="G79" s="9">
+        <f t="shared" si="4"/>
+        <v>122.13645931296026</v>
+      </c>
+      <c r="H79" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I79" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J79" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="80" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D80" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E80" s="1">
+        <v>2022</v>
+      </c>
+      <c r="F80" s="9">
+        <f t="shared" si="3"/>
+        <v>124.41811581873506</v>
+      </c>
+      <c r="G80" s="9">
+        <f t="shared" si="4"/>
+        <v>124.41811581873506</v>
+      </c>
+      <c r="H80" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I80" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J80" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="81" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D81" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E81" s="1">
+        <v>2023</v>
+      </c>
+      <c r="F81" s="9">
+        <f t="shared" si="3"/>
+        <v>121.11360025038407</v>
+      </c>
+      <c r="G81" s="9">
+        <f t="shared" si="4"/>
+        <v>121.11360025038407</v>
+      </c>
+      <c r="H81" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I81" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J81" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="82" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D82" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E82" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F82" s="9">
+        <f t="shared" si="3"/>
+        <v>117.99109945842528</v>
+      </c>
+      <c r="G82" s="9">
+        <f t="shared" si="4"/>
+        <v>117.99109945842528</v>
+      </c>
+      <c r="H82" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I82" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J82" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="83" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D83" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E83" s="1">
+        <v>2025</v>
+      </c>
+      <c r="F83" s="9">
+        <f t="shared" si="3"/>
+        <v>115.85212149427029</v>
+      </c>
+      <c r="G83" s="9">
+        <f t="shared" si="4"/>
+        <v>115.85212149427029</v>
+      </c>
+      <c r="H83" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I83" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J83" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="84" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D84" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E84" s="1">
+        <v>2026</v>
+      </c>
+      <c r="F84" s="9">
+        <f t="shared" si="3"/>
+        <v>114.12044665348095</v>
+      </c>
+      <c r="G84" s="9">
+        <f t="shared" si="4"/>
+        <v>114.12044665348095</v>
+      </c>
+      <c r="H84" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I84" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J84" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="85" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D85" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E85" s="1">
+        <v>2027</v>
+      </c>
+      <c r="F85" s="9">
+        <f t="shared" si="3"/>
+        <v>112.70073336603708</v>
+      </c>
+      <c r="G85" s="9">
+        <f t="shared" si="4"/>
+        <v>112.70073336603708</v>
+      </c>
+      <c r="H85" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I85" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J85" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="86" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D86" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E86" s="1">
+        <v>2028</v>
+      </c>
+      <c r="F86" s="9">
+        <f t="shared" si="3"/>
+        <v>111.50142979126321</v>
+      </c>
+      <c r="G86" s="9">
+        <f t="shared" si="4"/>
+        <v>111.50142979126321</v>
+      </c>
+      <c r="H86" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I86" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J86" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="87" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D87" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E87" s="1">
+        <v>2029</v>
+      </c>
+      <c r="F87" s="9">
+        <f t="shared" si="3"/>
+        <v>110.30737579982764</v>
+      </c>
+      <c r="G87" s="9">
+        <f t="shared" si="4"/>
+        <v>110.30737579982764</v>
+      </c>
+      <c r="H87" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I87" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J87" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="88" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D88" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E88" s="1">
+        <v>2030</v>
+      </c>
+      <c r="F88" s="9">
+        <f t="shared" si="3"/>
+        <v>109.12143458640294</v>
+      </c>
+      <c r="G88" s="9">
+        <f t="shared" si="4"/>
+        <v>109.12143458640294</v>
+      </c>
+      <c r="H88" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I88" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J88" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="89" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D89" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E89" s="1">
+        <v>2031</v>
+      </c>
+      <c r="F89" s="9">
+        <f t="shared" si="3"/>
+        <v>112.6917989342659</v>
+      </c>
+      <c r="G89" s="9">
+        <f t="shared" si="4"/>
+        <v>112.6917989342659</v>
+      </c>
+      <c r="H89" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I89" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J89" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="90" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D90" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E90" s="1">
+        <v>2032</v>
+      </c>
+      <c r="F90" s="9">
+        <f t="shared" si="3"/>
+        <v>108.57365134801012</v>
+      </c>
+      <c r="G90" s="9">
+        <f t="shared" si="4"/>
+        <v>108.57365134801012</v>
+      </c>
+      <c r="H90" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I90" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J90" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="91" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D91" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E91" s="1">
+        <v>2033</v>
+      </c>
+      <c r="F91" s="9">
+        <f t="shared" si="3"/>
+        <v>107.50918197181177</v>
+      </c>
+      <c r="G91" s="9">
+        <f t="shared" si="4"/>
+        <v>107.50918197181177</v>
+      </c>
+      <c r="H91" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I91" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J91" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="92" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D92" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E92" s="1">
+        <v>2034</v>
+      </c>
+      <c r="F92" s="9">
+        <f t="shared" si="3"/>
+        <v>106.46293332514962</v>
+      </c>
+      <c r="G92" s="9">
+        <f t="shared" si="4"/>
+        <v>106.46293332514962</v>
+      </c>
+      <c r="H92" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I92" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J92" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="93" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D93" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E93" s="1">
+        <v>2035</v>
+      </c>
+      <c r="F93" s="9">
+        <f t="shared" si="3"/>
+        <v>105.37309921224487</v>
+      </c>
+      <c r="G93" s="9">
+        <f t="shared" si="4"/>
+        <v>105.37309921224487</v>
+      </c>
+      <c r="H93" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I93" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J93" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="94" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D94" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E94" s="1">
+        <v>2036</v>
+      </c>
+      <c r="F94" s="9">
+        <f t="shared" si="3"/>
+        <v>104.26749833554788</v>
+      </c>
+      <c r="G94" s="9">
+        <f t="shared" si="4"/>
+        <v>104.26749833554788</v>
+      </c>
+      <c r="H94" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I94" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J94" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="95" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D95" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E95" s="1">
+        <v>2037</v>
+      </c>
+      <c r="F95" s="9">
+        <f t="shared" si="3"/>
+        <v>103.1450162587365</v>
+      </c>
+      <c r="G95" s="9">
+        <f t="shared" si="4"/>
+        <v>103.1450162587365</v>
+      </c>
+      <c r="H95" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I95" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J95" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="96" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D96" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E96" s="1">
+        <v>2038</v>
+      </c>
+      <c r="F96" s="9">
+        <f t="shared" si="3"/>
+        <v>102.01713630177635</v>
+      </c>
+      <c r="G96" s="9">
+        <f t="shared" si="4"/>
+        <v>102.01713630177635</v>
+      </c>
+      <c r="H96" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I96" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J96" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="97" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D97" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E97" s="1">
+        <v>2039</v>
+      </c>
+      <c r="F97" s="9">
+        <f t="shared" si="3"/>
+        <v>100.85666552681393</v>
+      </c>
+      <c r="G97" s="9">
+        <f t="shared" si="4"/>
+        <v>100.85666552681393</v>
+      </c>
+      <c r="H97" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I97" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J97" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="98" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D98" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E98" s="1">
+        <v>2040</v>
+      </c>
+      <c r="F98" s="9">
+        <f t="shared" si="3"/>
+        <v>99.684506408872593</v>
+      </c>
+      <c r="G98" s="9">
+        <f t="shared" si="4"/>
+        <v>99.684506408872593</v>
+      </c>
+      <c r="H98" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I98" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J98" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="99" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D99" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E99" s="1">
+        <v>2045</v>
+      </c>
+      <c r="F99" s="9">
+        <f t="shared" si="3"/>
+        <v>170.73963988979949</v>
+      </c>
+      <c r="G99" s="9">
+        <f t="shared" si="4"/>
+        <v>170.73963988979949</v>
+      </c>
+      <c r="H99" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I99" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J99" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="100" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D100" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E100" s="1">
+        <v>2050</v>
+      </c>
+      <c r="F100" s="9">
+        <f t="shared" si="3"/>
+        <v>144.24052199364721</v>
+      </c>
+      <c r="G100" s="9">
+        <f t="shared" si="4"/>
+        <v>144.24052199364721</v>
+      </c>
+      <c r="H100" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I100" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J100" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="101" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D101" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E101" s="1">
+        <v>2055</v>
+      </c>
+      <c r="F101" s="9">
+        <f t="shared" si="3"/>
+        <v>134.77041890705948</v>
+      </c>
+      <c r="G101" s="9">
+        <f t="shared" si="4"/>
+        <v>134.77041890705948</v>
+      </c>
+      <c r="H101" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I101" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J101" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="102" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D102" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E102" s="1">
+        <v>2060</v>
+      </c>
+      <c r="F102" s="9">
+        <f t="shared" si="3"/>
+        <v>125.0570287768019</v>
+      </c>
+      <c r="G102" s="9">
+        <f t="shared" si="4"/>
+        <v>125.0570287768019</v>
+      </c>
+      <c r="H102" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I102" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J102" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="103" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D103" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E103" s="1">
+        <v>2065</v>
+      </c>
+      <c r="F103" s="9">
+        <f t="shared" si="3"/>
+        <v>125.52674406686971</v>
+      </c>
+      <c r="G103" s="9">
+        <f t="shared" si="4"/>
+        <v>125.52674406686971</v>
+      </c>
+      <c r="H103" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I103" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J103" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="104" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D104" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E104" s="1">
+        <v>2070</v>
+      </c>
+      <c r="F104" s="9">
+        <f t="shared" si="3"/>
+        <v>124.95012745649218</v>
+      </c>
+      <c r="G104" s="9">
+        <f t="shared" si="4"/>
+        <v>124.95012745649218</v>
+      </c>
+      <c r="H104" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I104" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J104" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="105" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D105" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E105" s="1">
+        <v>2075</v>
+      </c>
+      <c r="F105" s="9">
+        <f t="shared" si="3"/>
+        <v>125.45667495984314</v>
+      </c>
+      <c r="G105" s="9">
+        <f t="shared" si="4"/>
+        <v>125.45667495984314</v>
+      </c>
+      <c r="H105" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I105" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J105" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="106" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D106" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E106" s="1">
+        <v>2080</v>
+      </c>
+      <c r="F106" s="9">
+        <f t="shared" si="3"/>
+        <v>126.40434741592387</v>
+      </c>
+      <c r="G106" s="9">
+        <f t="shared" si="4"/>
+        <v>126.40434741592387</v>
+      </c>
+      <c r="H106" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I106" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J106" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="107" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D107" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E107" s="1">
+        <v>2085</v>
+      </c>
+      <c r="F107" s="9">
+        <f t="shared" si="3"/>
+        <v>126.65940700266059</v>
+      </c>
+      <c r="G107" s="9">
+        <f t="shared" si="4"/>
+        <v>126.65940700266059</v>
+      </c>
+      <c r="H107" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I107" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J107" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="108" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D108" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E108" s="1">
+        <v>2090</v>
+      </c>
+      <c r="F108" s="9">
+        <f t="shared" si="3"/>
+        <v>125.70528832857735</v>
+      </c>
+      <c r="G108" s="9">
+        <f t="shared" si="4"/>
+        <v>125.70528832857735</v>
+      </c>
+      <c r="H108" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I108" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J108" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="109" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D109" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E109" s="1">
+        <v>2095</v>
+      </c>
+      <c r="F109" s="9">
+        <f t="shared" si="3"/>
+        <v>123.4487141585752</v>
+      </c>
+      <c r="G109" s="9">
+        <f t="shared" si="4"/>
+        <v>123.4487141585752</v>
+      </c>
+      <c r="H109" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I109" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J109" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="110" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D110" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E110" s="1">
+        <v>2100</v>
+      </c>
+      <c r="F110" s="9">
+        <f t="shared" si="3"/>
+        <v>120.64007290651311</v>
+      </c>
+      <c r="G110" s="9">
+        <f t="shared" si="4"/>
+        <v>120.64007290651311</v>
+      </c>
+      <c r="H110" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I110" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J110" s="20" t="s">
+        <v>63</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>